<commit_message>
Update Excel and fixing SCD0026-009 (Belum Semua Ke Update)
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0004-006 - Upload List File Expired 1 Bulan.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0004-006 - Upload List File Expired 1 Bulan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B759F3AD-D453-4D62-A3A6-E7E7676A43E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539422CD-1459-4C15-BC2C-BDB56C16AFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{9AD3C288-A382-489C-B5A3-5612378D2CD7}"/>
   </bookViews>
@@ -154,9 +154,6 @@
     <t>Menampilkan list data yang sudah expired</t>
   </si>
   <si>
-    <t>Testing UFT SCD0017</t>
-  </si>
-  <si>
     <t>FileDist18042022_9.dat</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>SCD0004-006</t>
+  </si>
+  <si>
+    <t>Testing UFT SCD0004-006</t>
   </si>
 </sst>
 </file>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9BE5456-1E7C-409D-93CC-40083DA405EA}">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,21 +689,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="F2" s="3">
         <v>52326</v>
@@ -722,13 +722,13 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="7"/>
       <c r="R2" s="4"/>
@@ -748,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -757,7 +757,7 @@
         <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="3">
         <v>49998</v>
@@ -796,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -805,7 +805,7 @@
         <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -827,11 +827,11 @@
       <c r="Q4" s="7"/>
       <c r="R4" s="5" t="str">
         <f>"USE DigisalesNew; SELECT * FROM dbo.MasterFile WHERE keterangan ='"&amp;N2&amp;"'"</f>
-        <v>USE DigisalesNew; SELECT * FROM dbo.MasterFile WHERE keterangan ='Testing UFT SCD0017'</v>
+        <v>USE DigisalesNew; SELECT * FROM dbo.MasterFile WHERE keterangan ='Testing UFT SCD0004-006'</v>
       </c>
       <c r="S4" s="5" t="str">
         <f ca="1">"USE DigisalesNew; UPDATE dbo.MasterFile SET ExpiredDate = '"&amp;TEXT(TODAY()-31,"yyyy-mm-dd")&amp;"' WHERE keterangan = '"&amp;N2&amp;"'"</f>
-        <v>USE DigisalesNew; UPDATE dbo.MasterFile SET ExpiredDate = '2022-10-02' WHERE keterangan = 'Testing UFT SCD0017'</v>
+        <v>USE DigisalesNew; UPDATE dbo.MasterFile SET ExpiredDate = '2022-10-04' WHERE keterangan = 'Testing UFT SCD0004-006'</v>
       </c>
       <c r="T4" s="4"/>
       <c r="U4" s="4" t="str">
@@ -856,7 +856,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>20</v>
@@ -865,7 +865,7 @@
         <v>32</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="3">
         <v>52326</v>
@@ -904,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>20</v>
@@ -913,7 +913,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6" s="3">
         <v>49998</v>
@@ -952,7 +952,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>20</v>
@@ -961,7 +961,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -982,7 +982,7 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>

</xml_diff>